<commit_message>
fix over temp.fix usart1 error, not test yet
</commit_message>
<xml_diff>
--- a/FWG1_110/app/project/MDK_V5/AT32F415RBT7_WorkBench_analysis.xlsx
+++ b/FWG1_110/app/project/MDK_V5/AT32F415RBT7_WorkBench_analysis.xlsx
@@ -15,12 +15,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
   <si>
     <t>AT32F415RBT7_WorkBench</t>
   </si>
   <si>
-    <t>lto-llvm-e871cb.o</t>
+    <t>lto-llvm-b4bafb.o</t>
   </si>
   <si>
     <t>startup_at32f415.o</t>
@@ -35,6 +35,9 @@
     <t>dmul.o</t>
   </si>
   <si>
+    <t>ddiv.o</t>
+  </si>
+  <si>
     <t>mc_w.l</t>
   </si>
   <si>
@@ -42,6 +45,9 @@
   </si>
   <si>
     <t>fadd.o</t>
+  </si>
+  <si>
+    <t>fdiv.o</t>
   </si>
   <si>
     <t>fepilogue.o</t>
@@ -227,16 +233,16 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>ram_percent!$A$3:$A$33</c:f>
+              <c:f>ram_percent!$A$3:$A$35</c:f>
               <c:strCache>
-                <c:ptCount val="31"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
-                  <c:v>lto-llvm-e871cb.o</c:v>
+                  <c:v>lto-llvm-b4bafb.o</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>startup_at32f415.o</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="32">
                   <c:v>Totals</c:v>
                 </c:pt>
               </c:strCache>
@@ -244,17 +250,17 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ram_percent!$B$3:$B$33</c:f>
+              <c:f>ram_percent!$B$3:$B$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
-                  <c:v>92.83314514160156</c:v>
+                  <c:v>86.61175537109375</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.166853427886963</c:v>
-                </c:pt>
-                <c:pt idx="30">
+                  <c:v>13.38824653625488</c:v>
+                </c:pt>
+                <c:pt idx="32">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -322,11 +328,11 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>flash_percent!$A$3:$A$33</c:f>
+              <c:f>flash_percent!$A$3:$A$35</c:f>
               <c:strCache>
-                <c:ptCount val="31"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
-                  <c:v>lto-llvm-e871cb.o</c:v>
+                  <c:v>lto-llvm-b4bafb.o</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>mf_w.l</c:v>
@@ -341,81 +347,87 @@
                   <c:v>dmul.o</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>ddiv.o</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>mc_w.l</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>depilogue.o</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>fadd.o</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
+                  <c:v>fdiv.o</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>fepilogue.o</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>fmul.o</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>dfixi.o</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>dfixui.o</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>ffixui.o</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
                   <c:v>memseta.o</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="16">
                   <c:v>llsshr.o</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="17">
                   <c:v>init.o</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="18">
                   <c:v>dflti.o</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="19">
                   <c:v>llushr.o</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="20">
                   <c:v>llshl.o</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="21">
                   <c:v>handlers.o</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="22">
                   <c:v>fcmplt.o</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="23">
                   <c:v>fcmple.o</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="24">
                   <c:v>fcmpgt.o</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="25">
                   <c:v>fcmpge.o</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="26">
                   <c:v>dfltui.o</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="27">
                   <c:v>fflti.o</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="28">
                   <c:v>ffltui.o</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="29">
                   <c:v>entry9a.o</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="30">
                   <c:v>entry2.o</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="31">
                   <c:v>entry5.o</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="32">
                   <c:v>Totals</c:v>
                 </c:pt>
               </c:strCache>
@@ -423,101 +435,107 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>flash_percent!$B$3:$B$33</c:f>
+              <c:f>flash_percent!$B$3:$B$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
-                  <c:v>94.32582092285156</c:v>
+                  <c:v>89.45915985107422</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.209599733352661</c:v>
+                  <c:v>4.283676624298096</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.6007256507873535</c:v>
+                  <c:v>0.9446535706520081</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.4966395199298859</c:v>
+                  <c:v>0.7809759974479675</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.3390233814716339</c:v>
+                  <c:v>0.5331213474273682</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.3271278142929077</c:v>
+                  <c:v>0.5190918445587158</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.2765716910362244</c:v>
+                  <c:v>0.5144153237342835</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.2617022395133972</c:v>
+                  <c:v>0.434914767742157</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.1635639071464539</c:v>
+                  <c:v>0.4115322530269623</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.1486944556236267</c:v>
+                  <c:v>0.2899431884288788</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.09219056367874146</c:v>
+                  <c:v>0.2572076618671417</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.07434722781181335</c:v>
+                  <c:v>0.233825147151947</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.0594777837395668</c:v>
+                  <c:v>0.1449715942144394</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.0535300076007843</c:v>
+                  <c:v>0.1169125735759735</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.0535300076007843</c:v>
+                  <c:v>0.09353005886077881</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.0535300076007843</c:v>
+                  <c:v>0.08417705446481705</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.05055611580610275</c:v>
+                  <c:v>0.08417705446481705</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.0475822277367115</c:v>
+                  <c:v>0.08417705446481705</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.04460833966732025</c:v>
+                  <c:v>0.07950054854154587</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.04460833966732025</c:v>
+                  <c:v>0.07482405006885529</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.0416344478726387</c:v>
+                  <c:v>0.07014754414558411</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.0416344478726387</c:v>
+                  <c:v>0.07014754414558411</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.0416344478726387</c:v>
+                  <c:v>0.06547103822231293</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.0416344478726387</c:v>
+                  <c:v>0.06547103822231293</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.03866055980324745</c:v>
+                  <c:v>0.06547103822231293</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.02676500380039215</c:v>
+                  <c:v>0.06547103822231293</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.0148694459348917</c:v>
+                  <c:v>0.06079453602433205</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.01189555693417788</c:v>
+                  <c:v>0.04208852723240852</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.01189555693417788</c:v>
+                  <c:v>0.0233825147151947</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.005947778467088938</c:v>
+                  <c:v>0.01870601251721382</c:v>
                 </c:pt>
                 <c:pt idx="30">
+                  <c:v>0.01870601251721382</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.009353006258606911</c:v>
+                </c:pt>
+                <c:pt idx="32">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -622,8 +640,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:H33" totalsRowCount="1">
-  <autoFilter ref="A2:H32"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:H35" totalsRowCount="1">
+  <autoFilter ref="A2:H34"/>
   <tableColumns count="8">
     <tableColumn id="1" name="File_name" totalsRowLabel="Totals"/>
     <tableColumn id="2" name="ram_percent" totalsRowFunction="sum"/>
@@ -639,8 +657,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:H33" totalsRowCount="1">
-  <autoFilter ref="A2:H32"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:H35" totalsRowCount="1">
+  <autoFilter ref="A2:H34"/>
   <tableColumns count="8">
     <tableColumn id="1" name="File_name" totalsRowLabel="Totals"/>
     <tableColumn id="2" name="flash_percent" totalsRowFunction="sum"/>
@@ -940,7 +958,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -956,28 +974,28 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -985,25 +1003,25 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>92.83314514160156</v>
+        <v>86.61175537109375</v>
       </c>
       <c r="C3" s="1">
-        <v>13264</v>
+        <v>13249</v>
       </c>
       <c r="D3" s="1">
-        <v>63436</v>
+        <v>38259</v>
       </c>
       <c r="E3" s="1">
-        <v>63174</v>
+        <v>37978</v>
       </c>
       <c r="F3" s="1">
-        <v>130</v>
+        <v>148</v>
       </c>
       <c r="G3" s="1">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H3" s="1">
-        <v>13132</v>
+        <v>13116</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1011,10 +1029,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>7.166853427886963</v>
+        <v>13.38824653625488</v>
       </c>
       <c r="C4" s="1">
-        <v>1024</v>
+        <v>2048</v>
       </c>
       <c r="D4" s="1">
         <v>404</v>
@@ -1029,38 +1047,38 @@
         <v>0</v>
       </c>
       <c r="H4" s="1">
-        <v>1024</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B33">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35">
         <f>SUBTOTAL(109,[ram_percent])</f>
         <v>0</v>
       </c>
-      <c r="C33">
+      <c r="C35">
         <f>SUBTOTAL(109,[ram])</f>
         <v>0</v>
       </c>
-      <c r="D33">
+      <c r="D35">
         <f>SUBTOTAL(109,[flash])</f>
         <v>0</v>
       </c>
-      <c r="E33">
+      <c r="E35">
         <f>SUBTOTAL(109,[Code])</f>
         <v>0</v>
       </c>
-      <c r="F33">
+      <c r="F35">
         <f>SUBTOTAL(109,[RO_data])</f>
         <v>0</v>
       </c>
-      <c r="G33">
+      <c r="G35">
         <f>SUBTOTAL(109,[RW_data])</f>
         <v>0</v>
       </c>
-      <c r="H33">
+      <c r="H35">
         <f>SUBTOTAL(109,[ZI_data])</f>
         <v>0</v>
       </c>
@@ -1076,7 +1094,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1092,28 +1110,28 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" t="s">
         <v>40</v>
       </c>
-      <c r="C2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" t="s">
-        <v>38</v>
-      </c>
       <c r="H2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1121,25 +1139,25 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>94.32582092285156</v>
+        <v>89.45915985107422</v>
       </c>
       <c r="C3" s="1">
-        <v>63436</v>
+        <v>38259</v>
       </c>
       <c r="D3" s="1">
-        <v>13264</v>
+        <v>13249</v>
       </c>
       <c r="E3" s="1">
-        <v>63174</v>
+        <v>37978</v>
       </c>
       <c r="F3" s="1">
-        <v>130</v>
+        <v>148</v>
       </c>
       <c r="G3" s="1">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H3" s="1">
-        <v>13132</v>
+        <v>13116</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1147,16 +1165,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>2.209599733352661</v>
+        <v>4.283676624298096</v>
       </c>
       <c r="C4" s="1">
-        <v>1486</v>
+        <v>1832</v>
       </c>
       <c r="D4" s="1">
         <v>0</v>
       </c>
       <c r="E4" s="1">
-        <v>1486</v>
+        <v>1832</v>
       </c>
       <c r="F4" s="1">
         <v>0</v>
@@ -1173,13 +1191,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="2">
-        <v>0.6007256507873535</v>
+        <v>0.9446535706520081</v>
       </c>
       <c r="C5" s="1">
         <v>404</v>
       </c>
       <c r="D5" s="1">
-        <v>1024</v>
+        <v>2048</v>
       </c>
       <c r="E5" s="1">
         <v>36</v>
@@ -1191,7 +1209,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="1">
-        <v>1024</v>
+        <v>2048</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1199,7 +1217,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2">
-        <v>0.4966395199298859</v>
+        <v>0.7809759974479675</v>
       </c>
       <c r="C6" s="1">
         <v>334</v>
@@ -1225,7 +1243,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="2">
-        <v>0.3390233814716339</v>
+        <v>0.5331213474273682</v>
       </c>
       <c r="C7" s="1">
         <v>228</v>
@@ -1251,16 +1269,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="2">
-        <v>0.3271278142929077</v>
+        <v>0.5190918445587158</v>
       </c>
       <c r="C8" s="1">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D8" s="1">
         <v>0</v>
       </c>
       <c r="E8" s="1">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="F8" s="1">
         <v>0</v>
@@ -1277,16 +1295,16 @@
         <v>7</v>
       </c>
       <c r="B9" s="2">
-        <v>0.2765716910362244</v>
+        <v>0.5144153237342835</v>
       </c>
       <c r="C9" s="1">
-        <v>186</v>
+        <v>220</v>
       </c>
       <c r="D9" s="1">
         <v>0</v>
       </c>
       <c r="E9" s="1">
-        <v>186</v>
+        <v>220</v>
       </c>
       <c r="F9" s="1">
         <v>0</v>
@@ -1303,16 +1321,16 @@
         <v>8</v>
       </c>
       <c r="B10" s="2">
-        <v>0.2617022395133972</v>
+        <v>0.434914767742157</v>
       </c>
       <c r="C10" s="1">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="D10" s="1">
         <v>0</v>
       </c>
       <c r="E10" s="1">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="F10" s="1">
         <v>0</v>
@@ -1329,16 +1347,16 @@
         <v>9</v>
       </c>
       <c r="B11" s="2">
-        <v>0.1635639071464539</v>
+        <v>0.4115322530269623</v>
       </c>
       <c r="C11" s="1">
-        <v>110</v>
+        <v>176</v>
       </c>
       <c r="D11" s="1">
         <v>0</v>
       </c>
       <c r="E11" s="1">
-        <v>110</v>
+        <v>176</v>
       </c>
       <c r="F11" s="1">
         <v>0</v>
@@ -1355,16 +1373,16 @@
         <v>10</v>
       </c>
       <c r="B12" s="2">
-        <v>0.1486944556236267</v>
+        <v>0.2899431884288788</v>
       </c>
       <c r="C12" s="1">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="D12" s="1">
         <v>0</v>
       </c>
       <c r="E12" s="1">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="F12" s="1">
         <v>0</v>
@@ -1381,16 +1399,16 @@
         <v>11</v>
       </c>
       <c r="B13" s="2">
-        <v>0.09219056367874146</v>
+        <v>0.2572076618671417</v>
       </c>
       <c r="C13" s="1">
-        <v>62</v>
+        <v>110</v>
       </c>
       <c r="D13" s="1">
         <v>0</v>
       </c>
       <c r="E13" s="1">
-        <v>62</v>
+        <v>110</v>
       </c>
       <c r="F13" s="1">
         <v>0</v>
@@ -1407,16 +1425,16 @@
         <v>12</v>
       </c>
       <c r="B14" s="2">
-        <v>0.07434722781181335</v>
+        <v>0.233825147151947</v>
       </c>
       <c r="C14" s="1">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D14" s="1">
         <v>0</v>
       </c>
       <c r="E14" s="1">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="F14" s="1">
         <v>0</v>
@@ -1433,16 +1451,16 @@
         <v>13</v>
       </c>
       <c r="B15" s="2">
-        <v>0.0594777837395668</v>
+        <v>0.1449715942144394</v>
       </c>
       <c r="C15" s="1">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="D15" s="1">
         <v>0</v>
       </c>
       <c r="E15" s="1">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="F15" s="1">
         <v>0</v>
@@ -1459,16 +1477,16 @@
         <v>14</v>
       </c>
       <c r="B16" s="2">
-        <v>0.0535300076007843</v>
+        <v>0.1169125735759735</v>
       </c>
       <c r="C16" s="1">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="D16" s="1">
         <v>0</v>
       </c>
       <c r="E16" s="1">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="F16" s="1">
         <v>0</v>
@@ -1485,16 +1503,16 @@
         <v>15</v>
       </c>
       <c r="B17" s="2">
-        <v>0.0535300076007843</v>
+        <v>0.09353005886077881</v>
       </c>
       <c r="C17" s="1">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D17" s="1">
         <v>0</v>
       </c>
       <c r="E17" s="1">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F17" s="1">
         <v>0</v>
@@ -1511,7 +1529,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="2">
-        <v>0.0535300076007843</v>
+        <v>0.08417705446481705</v>
       </c>
       <c r="C18" s="1">
         <v>36</v>
@@ -1537,16 +1555,16 @@
         <v>17</v>
       </c>
       <c r="B19" s="2">
-        <v>0.05055611580610275</v>
+        <v>0.08417705446481705</v>
       </c>
       <c r="C19" s="1">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D19" s="1">
         <v>0</v>
       </c>
       <c r="E19" s="1">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F19" s="1">
         <v>0</v>
@@ -1563,16 +1581,16 @@
         <v>18</v>
       </c>
       <c r="B20" s="2">
-        <v>0.0475822277367115</v>
+        <v>0.08417705446481705</v>
       </c>
       <c r="C20" s="1">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D20" s="1">
         <v>0</v>
       </c>
       <c r="E20" s="1">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="F20" s="1">
         <v>0</v>
@@ -1589,16 +1607,16 @@
         <v>19</v>
       </c>
       <c r="B21" s="2">
-        <v>0.04460833966732025</v>
+        <v>0.07950054854154587</v>
       </c>
       <c r="C21" s="1">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D21" s="1">
         <v>0</v>
       </c>
       <c r="E21" s="1">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F21" s="1">
         <v>0</v>
@@ -1615,16 +1633,16 @@
         <v>20</v>
       </c>
       <c r="B22" s="2">
-        <v>0.04460833966732025</v>
+        <v>0.07482405006885529</v>
       </c>
       <c r="C22" s="1">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D22" s="1">
         <v>0</v>
       </c>
       <c r="E22" s="1">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F22" s="1">
         <v>0</v>
@@ -1641,16 +1659,16 @@
         <v>21</v>
       </c>
       <c r="B23" s="2">
-        <v>0.0416344478726387</v>
+        <v>0.07014754414558411</v>
       </c>
       <c r="C23" s="1">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D23" s="1">
         <v>0</v>
       </c>
       <c r="E23" s="1">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F23" s="1">
         <v>0</v>
@@ -1667,16 +1685,16 @@
         <v>22</v>
       </c>
       <c r="B24" s="2">
-        <v>0.0416344478726387</v>
+        <v>0.07014754414558411</v>
       </c>
       <c r="C24" s="1">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D24" s="1">
         <v>0</v>
       </c>
       <c r="E24" s="1">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F24" s="1">
         <v>0</v>
@@ -1693,7 +1711,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="2">
-        <v>0.0416344478726387</v>
+        <v>0.06547103822231293</v>
       </c>
       <c r="C25" s="1">
         <v>28</v>
@@ -1719,7 +1737,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="2">
-        <v>0.0416344478726387</v>
+        <v>0.06547103822231293</v>
       </c>
       <c r="C26" s="1">
         <v>28</v>
@@ -1745,16 +1763,16 @@
         <v>25</v>
       </c>
       <c r="B27" s="2">
-        <v>0.03866055980324745</v>
+        <v>0.06547103822231293</v>
       </c>
       <c r="C27" s="1">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D27" s="1">
         <v>0</v>
       </c>
       <c r="E27" s="1">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F27" s="1">
         <v>0</v>
@@ -1771,16 +1789,16 @@
         <v>26</v>
       </c>
       <c r="B28" s="2">
-        <v>0.02676500380039215</v>
+        <v>0.06547103822231293</v>
       </c>
       <c r="C28" s="1">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="D28" s="1">
         <v>0</v>
       </c>
       <c r="E28" s="1">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="F28" s="1">
         <v>0</v>
@@ -1797,16 +1815,16 @@
         <v>27</v>
       </c>
       <c r="B29" s="2">
-        <v>0.0148694459348917</v>
+        <v>0.06079453602433205</v>
       </c>
       <c r="C29" s="1">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="D29" s="1">
         <v>0</v>
       </c>
       <c r="E29" s="1">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="F29" s="1">
         <v>0</v>
@@ -1823,16 +1841,16 @@
         <v>28</v>
       </c>
       <c r="B30" s="2">
-        <v>0.01189555693417788</v>
+        <v>0.04208852723240852</v>
       </c>
       <c r="C30" s="1">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="D30" s="1">
         <v>0</v>
       </c>
       <c r="E30" s="1">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="F30" s="1">
         <v>0</v>
@@ -1849,16 +1867,16 @@
         <v>29</v>
       </c>
       <c r="B31" s="2">
-        <v>0.01189555693417788</v>
+        <v>0.0233825147151947</v>
       </c>
       <c r="C31" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D31" s="1">
         <v>0</v>
       </c>
       <c r="E31" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F31" s="1">
         <v>0</v>
@@ -1875,56 +1893,108 @@
         <v>30</v>
       </c>
       <c r="B32" s="2">
-        <v>0.005947778467088938</v>
+        <v>0.01870601251721382</v>
       </c>
       <c r="C32" s="1">
+        <v>8</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1">
+        <v>8</v>
+      </c>
+      <c r="F32" s="1">
+        <v>0</v>
+      </c>
+      <c r="G32" s="1">
+        <v>0</v>
+      </c>
+      <c r="H32" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="2">
+        <v>0.01870601251721382</v>
+      </c>
+      <c r="C33" s="1">
+        <v>8</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0</v>
+      </c>
+      <c r="E33" s="1">
+        <v>8</v>
+      </c>
+      <c r="F33" s="1">
+        <v>0</v>
+      </c>
+      <c r="G33" s="1">
+        <v>0</v>
+      </c>
+      <c r="H33" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" s="2">
+        <v>0.009353006258606911</v>
+      </c>
+      <c r="C34" s="1">
         <v>4</v>
       </c>
-      <c r="D32" s="1">
-        <v>0</v>
-      </c>
-      <c r="E32" s="1">
+      <c r="D34" s="1">
+        <v>0</v>
+      </c>
+      <c r="E34" s="1">
         <v>4</v>
       </c>
-      <c r="F32" s="1">
-        <v>0</v>
-      </c>
-      <c r="G32" s="1">
-        <v>0</v>
-      </c>
-      <c r="H32" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B33">
+      <c r="F34" s="1">
+        <v>0</v>
+      </c>
+      <c r="G34" s="1">
+        <v>0</v>
+      </c>
+      <c r="H34" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35">
         <f>SUBTOTAL(109,[flash_percent])</f>
         <v>0</v>
       </c>
-      <c r="C33">
+      <c r="C35">
         <f>SUBTOTAL(109,[flash])</f>
         <v>0</v>
       </c>
-      <c r="D33">
+      <c r="D35">
         <f>SUBTOTAL(109,[ram])</f>
         <v>0</v>
       </c>
-      <c r="E33">
+      <c r="E35">
         <f>SUBTOTAL(109,[Code])</f>
         <v>0</v>
       </c>
-      <c r="F33">
+      <c r="F35">
         <f>SUBTOTAL(109,[RO_data])</f>
         <v>0</v>
       </c>
-      <c r="G33">
+      <c r="G35">
         <f>SUBTOTAL(109,[RW_data])</f>
         <v>0</v>
       </c>
-      <c r="H33">
+      <c r="H35">
         <f>SUBTOTAL(109,[ZI_data])</f>
         <v>0</v>
       </c>

</xml_diff>